<commit_message>
Unit tests almost ready. Just one assert to be completed.
</commit_message>
<xml_diff>
--- a/BridgeCareApp/BridgeCareCore/DownloadTemplates/Scenario_treatmentSupersedeRules_template.xlsx
+++ b/BridgeCareApp/BridgeCareCore/DownloadTemplates/Scenario_treatmentSupersedeRules_template.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://appliedresearchassociates-my.sharepoint.us/personal/aborgaonkar_ara_com/Documents/Documents/iAM/Feature-Treatments Supersede Rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aborgaonkar\source\repos\Infrastructure Asset Management\BridgeCareApp\BridgeCareCore\DownloadTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{A8848B98-5825-4D8E-A38E-FDF44AF8171A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{260B3AA0-A8AF-4A0A-802F-2197AD70FF70}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34535B87-7C02-4958-B260-2F088B159B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="4215" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="County Maintenance - Superstruc" sheetId="1" r:id="rId1"/>
-    <sheet name="TreatmentSupesedeRules" sheetId="11" r:id="rId2"/>
+    <sheet name="Treatment Supersede Rules" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>